<commit_message>
fix the classifier issue of ASV
</commit_message>
<xml_diff>
--- a/methods_comp_packages.xlsx
+++ b/methods_comp_packages.xlsx
@@ -70,7 +70,7 @@
     <t>++</t>
   </si>
   <si>
-    <t>CLR/RCLR/CSS/GMPR/TMM/RLE/TSS</t>
+    <t>CLR/RCLR/CSS/GMPR/TMM/RLE/TSS/DESeq2/Wrench</t>
   </si>
   <si>
     <t>+++</t>
@@ -1139,14 +1139,14 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:K27"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="12.8888888888889" style="2" customWidth="1"/>
     <col min="2" max="2" width="31.1111111111111" style="2" customWidth="1"/>
-    <col min="3" max="3" width="35.4444444444444" style="2" customWidth="1"/>
+    <col min="3" max="3" width="44.6666666666667" style="2" customWidth="1"/>
     <col min="4" max="4" width="20" style="3" customWidth="1"/>
     <col min="5" max="5" width="17.6666666666667" style="3" customWidth="1"/>
     <col min="6" max="6" width="24.6666666666667" style="2" customWidth="1"/>

</xml_diff>